<commit_message>
test cases fixed and finished
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/Lab4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cameron/PycharmProjects/cs151-lab4-cameron_harry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD855A85-678C-0D4F-A767-FA0C68848C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B268010F-051A-3346-B557-87AC7646F4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Test Description</t>
   </si>
@@ -106,6 +106,24 @@
   </si>
   <si>
     <t>Green Package 3 months with additional 5 GB data</t>
+  </si>
+  <si>
+    <t>input: does user have coupon</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>purple</t>
   </si>
 </sst>
 </file>
@@ -220,9 +238,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -260,7 +278,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -366,7 +384,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -508,7 +526,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -519,7 +537,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -661,7 +679,9 @@
       <c r="D8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="F8" s="6" t="s">
         <v>18</v>
       </c>
@@ -670,52 +690,108 @@
       </c>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="46" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="31" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="4">
+        <f>C2*C9</f>
+        <v>99.98</v>
+      </c>
+      <c r="G9" s="4">
+        <f>C2*C9-20</f>
+        <v>79.98</v>
+      </c>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="46" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="31" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" ref="F10:F12" si="0">C3*C10</f>
+        <v>140</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" ref="G10:G11" si="1">C3*C10</f>
+        <v>140</v>
+      </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="46" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="31" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="B11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="0"/>
+        <v>199.9</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="1"/>
+        <v>199.9</v>
+      </c>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3">
+        <v>5</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="4">
+        <f>(C2*C12)+(D12*D2)</f>
+        <v>224.97</v>
+      </c>
+      <c r="G12" s="4">
+        <f>(C2*C12)+(D12*D2)-20</f>
+        <v>204.97</v>
+      </c>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>